<commit_message>
copy cell style between different types of files as possible as correctly
</commit_message>
<xml_diff>
--- a/tableio-excel/src/test/resources/info/informationsea/tableio/excel/test/cellltypes.xlsx
+++ b/tableio-excel/src/test/resources/info/informationsea/tableio/excel/test/cellltypes.xlsx
@@ -147,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -155,12 +155,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -174,6 +189,7 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -509,7 +525,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -550,7 +566,7 @@
       <c r="B3" s="11">
         <v>3.4</v>
       </c>
-      <c r="C3" t="b">
+      <c r="C3" s="13" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="str">

</xml_diff>